<commit_message>
comments added for todo
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -38,14 +38,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -536,7 +536,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>1.39</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -544,7 +544,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="2" t="n">
         <v>601.0700000000001</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -572,7 +572,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="2" t="n">
         <v>675.74</v>
       </c>
       <c r="L3" t="inlineStr">
@@ -648,7 +648,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="2" t="n">
         <v>444.2</v>
       </c>
       <c r="L6" t="inlineStr">
@@ -668,7 +668,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="F7" t="inlineStr">
@@ -708,7 +708,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="F9" t="inlineStr">
@@ -728,7 +728,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,7 +748,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="3" t="n">
         <v>2309.45</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -756,7 +756,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="K11" s="3" t="n">
         <v>1153.24</v>
       </c>
       <c r="L11" t="inlineStr">
@@ -792,7 +792,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K12" t="n">
+      <c r="K12" s="2" t="n">
         <v>799.01</v>
       </c>
       <c r="L12" t="inlineStr">
@@ -828,7 +828,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K13" t="n">
+      <c r="K13" s="2" t="n">
         <v>678.92</v>
       </c>
       <c r="L13" t="inlineStr">
@@ -872,7 +872,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="2" t="n">
         <v>549.92</v>
       </c>
       <c r="J14" t="inlineStr">
@@ -1036,7 +1036,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F21" t="inlineStr">
@@ -1056,7 +1056,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="3" t="n">
         <v>1.58</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -1168,7 +1168,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G26" s="3" t="n">
+      <c r="G26" s="2" t="n">
         <v>0.45</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -1188,7 +1188,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="E27" s="2" t="n">
         <v>0.19</v>
       </c>
       <c r="F27" t="inlineStr">
@@ -1196,7 +1196,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G27" s="3" t="n">
+      <c r="G27" s="2" t="n">
         <v>0.43</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -1216,7 +1216,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C28" s="3" t="n">
         <v>2.33</v>
       </c>
       <c r="D28" t="inlineStr">
@@ -1224,7 +1224,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="3" t="n">
         <v>2.52</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -1272,7 +1272,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" s="3" t="n">
         <v>2.75</v>
       </c>
       <c r="D30" t="inlineStr">
@@ -1280,7 +1280,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F30" t="inlineStr">
@@ -1288,7 +1288,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="3" t="n">
         <v>3.01</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -1308,7 +1308,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="3" t="n">
         <v>2.36</v>
       </c>
       <c r="D31" t="inlineStr">
@@ -1316,7 +1316,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G31" s="3" t="n">
         <v>2.58</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -1336,7 +1336,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="C32" s="3" t="n">
         <v>2.65</v>
       </c>
       <c r="D32" t="inlineStr">
@@ -1344,7 +1344,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G32" s="3" t="n">
         <v>2.84</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -1392,7 +1392,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="E34" s="3" t="n">
+      <c r="E34" s="2" t="n">
         <v>0.21</v>
       </c>
       <c r="F34" t="inlineStr">
@@ -1400,7 +1400,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="2" t="n">
         <v>522.3099999999999</v>
       </c>
       <c r="L34" t="inlineStr">
@@ -1440,7 +1440,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="D36" t="inlineStr">
@@ -1460,7 +1460,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="D37" t="inlineStr">
@@ -1468,7 +1468,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K37" t="n">
+      <c r="K37" s="2" t="n">
         <v>613.61</v>
       </c>
       <c r="L37" t="inlineStr">
@@ -1516,7 +1516,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K39" t="n">
+      <c r="K39" s="2" t="n">
         <v>665</v>
       </c>
       <c r="L39" t="inlineStr">
@@ -1592,7 +1592,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="2" t="n">
         <v>0.21</v>
       </c>
       <c r="F42" t="inlineStr">
@@ -1744,7 +1744,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G48" s="2" t="n">
+      <c r="G48" s="3" t="n">
         <v>1.52</v>
       </c>
       <c r="H48" t="inlineStr">
@@ -1752,7 +1752,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K48" t="n">
+      <c r="K48" s="2" t="n">
         <v>582.11</v>
       </c>
       <c r="L48" t="inlineStr">
@@ -1840,7 +1840,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E52" s="3" t="n">
+      <c r="E52" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F52" t="inlineStr">
@@ -1860,7 +1860,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E53" s="3" t="n">
+      <c r="E53" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F53" t="inlineStr">
@@ -1888,7 +1888,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I54" t="n">
+      <c r="I54" s="3" t="n">
         <v>2098.51</v>
       </c>
       <c r="J54" t="inlineStr">
@@ -1896,7 +1896,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K54" t="n">
+      <c r="K54" s="2" t="n">
         <v>907.65</v>
       </c>
       <c r="L54" t="inlineStr">
@@ -1916,7 +1916,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
+      <c r="C55" s="3" t="n">
         <v>1.68</v>
       </c>
       <c r="D55" t="inlineStr">
@@ -1924,7 +1924,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E55" s="3" t="n">
+      <c r="E55" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F55" t="inlineStr">
@@ -1932,7 +1932,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G55" s="2" t="n">
+      <c r="G55" s="3" t="n">
         <v>1.34</v>
       </c>
       <c r="H55" t="inlineStr">
@@ -1952,7 +1952,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
+      <c r="C56" s="3" t="n">
         <v>1.6</v>
       </c>
       <c r="D56" t="inlineStr">
@@ -1968,7 +1968,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G56" s="2" t="n">
+      <c r="G56" s="3" t="n">
         <v>1.26</v>
       </c>
       <c r="H56" t="inlineStr">
@@ -1988,7 +1988,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E57" s="3" t="n">
+      <c r="E57" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F57" t="inlineStr">
@@ -2044,7 +2044,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E59" s="3" t="n">
+      <c r="E59" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F59" t="inlineStr">
@@ -2072,7 +2072,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E60" s="3" t="n">
+      <c r="E60" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F60" t="inlineStr">
@@ -2100,7 +2100,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E61" s="3" t="n">
+      <c r="E61" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F61" t="inlineStr">
@@ -2108,7 +2108,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I61" t="n">
+      <c r="I61" s="2" t="n">
         <v>790.48</v>
       </c>
       <c r="J61" t="inlineStr">
@@ -2116,7 +2116,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K61" t="n">
+      <c r="K61" s="2" t="n">
         <v>986.17</v>
       </c>
       <c r="L61" t="inlineStr">
@@ -2180,7 +2180,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I63" t="n">
+      <c r="I63" s="2" t="n">
         <v>871.26</v>
       </c>
       <c r="J63" t="inlineStr">
@@ -2188,7 +2188,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K63" t="n">
+      <c r="K63" s="2" t="n">
         <v>660.51</v>
       </c>
       <c r="L63" t="inlineStr">
@@ -2216,7 +2216,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G64" s="2" t="n">
+      <c r="G64" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H64" t="inlineStr">
@@ -2256,7 +2256,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E66" s="3" t="n">
+      <c r="E66" s="2" t="n">
         <v>0.24</v>
       </c>
       <c r="F66" t="inlineStr">
@@ -2324,7 +2324,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K69" t="n">
+      <c r="K69" s="2" t="n">
         <v>423.92</v>
       </c>
       <c r="L69" t="inlineStr">
@@ -2372,7 +2372,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C71" s="3" t="n">
+      <c r="C71" s="2" t="n">
         <v>0.18</v>
       </c>
       <c r="D71" t="inlineStr">
@@ -2392,7 +2392,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C72" s="3" t="n">
+      <c r="C72" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="D72" t="inlineStr">
@@ -2412,7 +2412,7 @@
           <t>32</t>
         </is>
       </c>
-      <c r="E73" s="3" t="n">
+      <c r="E73" s="2" t="n">
         <v>0.21</v>
       </c>
       <c r="F73" t="inlineStr">
@@ -2432,7 +2432,7 @@
           <t>36</t>
         </is>
       </c>
-      <c r="C74" s="2" t="n">
+      <c r="C74" s="3" t="n">
         <v>1.01</v>
       </c>
       <c r="D74" t="inlineStr">
@@ -2468,7 +2468,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I75" t="n">
+      <c r="I75" s="2" t="n">
         <v>452.54</v>
       </c>
       <c r="J75" t="inlineStr">
@@ -2564,7 +2564,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C79" s="2" t="n">
+      <c r="C79" s="3" t="n">
         <v>1.33</v>
       </c>
       <c r="D79" t="inlineStr">
@@ -2572,7 +2572,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E79" s="2" t="n">
+      <c r="E79" s="3" t="n">
         <v>1.27</v>
       </c>
       <c r="F79" t="inlineStr">
@@ -2592,7 +2592,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="E80" s="3" t="n">
+      <c r="E80" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F80" t="inlineStr">
@@ -2612,7 +2612,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C81" s="2" t="n">
+      <c r="C81" s="3" t="n">
         <v>2.06</v>
       </c>
       <c r="D81" t="inlineStr">
@@ -2620,7 +2620,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G81" s="2" t="n">
+      <c r="G81" s="3" t="n">
         <v>1.86</v>
       </c>
       <c r="H81" t="inlineStr">
@@ -2640,7 +2640,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C82" s="2" t="n">
+      <c r="C82" s="3" t="n">
         <v>3.07</v>
       </c>
       <c r="D82" t="inlineStr">
@@ -2648,7 +2648,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E82" s="2" t="n">
+      <c r="E82" s="3" t="n">
         <v>3.11</v>
       </c>
       <c r="F82" t="inlineStr">
@@ -2668,7 +2668,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C83" s="2" t="n">
+      <c r="C83" s="3" t="n">
         <v>1.27</v>
       </c>
       <c r="D83" t="inlineStr">
@@ -2708,7 +2708,7 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E85" s="3" t="n">
+      <c r="E85" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="F85" t="inlineStr">
@@ -2716,7 +2716,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K85" t="n">
+      <c r="K85" s="2" t="n">
         <v>672.37</v>
       </c>
       <c r="L85" t="inlineStr">
@@ -2756,7 +2756,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E87" s="3" t="n">
+      <c r="E87" s="2" t="n">
         <v>0.18</v>
       </c>
       <c r="F87" t="inlineStr">
@@ -2776,7 +2776,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E88" s="3" t="n">
+      <c r="E88" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F88" t="inlineStr">
@@ -2784,7 +2784,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K88" t="n">
+      <c r="K88" s="2" t="n">
         <v>835.33</v>
       </c>
       <c r="L88" t="inlineStr">
@@ -2804,7 +2804,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E89" s="3" t="n">
+      <c r="E89" s="2" t="n">
         <v>0.24</v>
       </c>
       <c r="F89" t="inlineStr">
@@ -2824,7 +2824,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E90" s="3" t="n">
+      <c r="E90" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="F90" t="inlineStr">
@@ -2844,7 +2844,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E91" s="3" t="n">
+      <c r="E91" s="2" t="n">
         <v>0.22</v>
       </c>
       <c r="F91" t="inlineStr">

</xml_diff>

<commit_message>
fix: t_con_force is now correctly detected
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -38,14 +38,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -528,7 +528,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.46</v>
       </c>
       <c r="F2" t="inlineStr">
@@ -536,7 +536,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="2" t="n">
         <v>1.39</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -544,7 +544,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>601.0700000000001</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -564,7 +564,7 @@
           <t>02</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>0.29</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -572,7 +572,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="3" t="n">
         <v>675.74</v>
       </c>
       <c r="L3" t="inlineStr">
@@ -592,7 +592,7 @@
           <t>02</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>0.27</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -612,7 +612,7 @@
           <t>02</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>0.4</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -632,7 +632,7 @@
           <t>02</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>0.48</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -640,18 +640,10 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="F6" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>444.2</v>
-      </c>
-      <c r="L6" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -668,7 +660,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.2</v>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,7 +680,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.29</v>
       </c>
       <c r="F8" t="inlineStr">
@@ -708,7 +700,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>0.2</v>
       </c>
       <c r="F9" t="inlineStr">
@@ -728,7 +720,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,7 +740,7 @@
           <t>09</t>
         </is>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="2" t="n">
         <v>2309.45</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -756,7 +748,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="2" t="n">
         <v>1153.24</v>
       </c>
       <c r="L11" t="inlineStr">
@@ -784,7 +776,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <v>0.77</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -812,7 +804,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="3" t="n">
         <v>0.53</v>
       </c>
       <c r="F13" t="inlineStr">
@@ -820,7 +812,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <v>0.54</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -828,7 +820,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="K13" s="3" t="n">
         <v>678.92</v>
       </c>
       <c r="L13" t="inlineStr">
@@ -848,7 +840,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <v>0.39</v>
       </c>
       <c r="D14" t="inlineStr">
@@ -856,7 +848,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="3" t="n">
         <v>0.39</v>
       </c>
       <c r="F14" t="inlineStr">
@@ -864,7 +856,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <v>0.8100000000000001</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -872,7 +864,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <v>549.92</v>
       </c>
       <c r="J14" t="inlineStr">
@@ -892,7 +884,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <v>0.58</v>
       </c>
       <c r="D15" t="inlineStr">
@@ -900,7 +892,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <v>0.72</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -928,7 +920,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <v>0.68</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -948,7 +940,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="3" t="n">
         <v>0.36</v>
       </c>
       <c r="F17" t="inlineStr">
@@ -968,7 +960,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="3" t="n">
         <v>0.29</v>
       </c>
       <c r="D18" t="inlineStr">
@@ -988,7 +980,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="3" t="n">
         <v>0.29</v>
       </c>
       <c r="F19" t="inlineStr">
@@ -1008,7 +1000,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="3" t="n">
         <v>0.33</v>
       </c>
       <c r="F20" t="inlineStr">
@@ -1028,7 +1020,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="3" t="n">
         <v>0.68</v>
       </c>
       <c r="D21" t="inlineStr">
@@ -1036,7 +1028,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F21" t="inlineStr">
@@ -1056,7 +1048,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="2" t="n">
         <v>1.58</v>
       </c>
       <c r="D22" t="inlineStr">
@@ -1064,7 +1056,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="F22" t="inlineStr">
@@ -1092,7 +1084,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="3" t="n">
         <v>0.48</v>
       </c>
       <c r="D23" t="inlineStr">
@@ -1112,7 +1104,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="3" t="n">
         <v>0.4</v>
       </c>
       <c r="D24" t="inlineStr">
@@ -1120,7 +1112,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="3" t="n">
         <v>0.53</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -1140,7 +1132,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="3" t="n">
         <v>0.58</v>
       </c>
       <c r="D25" t="inlineStr">
@@ -1160,7 +1152,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="D26" t="inlineStr">
@@ -1168,7 +1160,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="3" t="n">
         <v>0.45</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -1188,7 +1180,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="3" t="n">
         <v>0.19</v>
       </c>
       <c r="F27" t="inlineStr">
@@ -1196,7 +1188,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="3" t="n">
         <v>0.43</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -1216,7 +1208,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="2" t="n">
         <v>2.33</v>
       </c>
       <c r="D28" t="inlineStr">
@@ -1224,7 +1216,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G28" s="3" t="n">
+      <c r="G28" s="2" t="n">
         <v>2.52</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -1244,7 +1236,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="3" t="n">
         <v>0.7</v>
       </c>
       <c r="D29" t="inlineStr">
@@ -1252,7 +1244,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="3" t="n">
         <v>0.85</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -1272,7 +1264,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="2" t="n">
         <v>2.75</v>
       </c>
       <c r="D30" t="inlineStr">
@@ -1280,7 +1272,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F30" t="inlineStr">
@@ -1288,7 +1280,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G30" s="3" t="n">
+      <c r="G30" s="2" t="n">
         <v>3.01</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -1308,7 +1300,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="2" t="n">
         <v>2.36</v>
       </c>
       <c r="D31" t="inlineStr">
@@ -1316,7 +1308,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G31" s="3" t="n">
+      <c r="G31" s="2" t="n">
         <v>2.58</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -1336,7 +1328,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="2" t="n">
         <v>2.65</v>
       </c>
       <c r="D32" t="inlineStr">
@@ -1344,7 +1336,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G32" s="3" t="n">
+      <c r="G32" s="2" t="n">
         <v>2.84</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -1364,7 +1356,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="3" t="n">
         <v>0.5</v>
       </c>
       <c r="F33" t="inlineStr">
@@ -1372,7 +1364,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G33" s="2" t="n">
+      <c r="G33" s="3" t="n">
         <v>0.51</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -1392,18 +1384,10 @@
           <t>14</t>
         </is>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" s="3" t="n">
         <v>0.21</v>
       </c>
       <c r="F34" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K34" s="2" t="n">
-        <v>522.3099999999999</v>
-      </c>
-      <c r="L34" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -1420,7 +1404,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="3" t="n">
         <v>0.26</v>
       </c>
       <c r="D35" t="inlineStr">
@@ -1440,7 +1424,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="D36" t="inlineStr">
@@ -1460,7 +1444,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="D37" t="inlineStr">
@@ -1468,7 +1452,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K37" s="2" t="n">
+      <c r="K37" s="3" t="n">
         <v>613.61</v>
       </c>
       <c r="L37" t="inlineStr">
@@ -1488,7 +1472,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="3" t="n">
         <v>0.34</v>
       </c>
       <c r="D38" t="inlineStr">
@@ -1508,7 +1492,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="3" t="n">
         <v>0.27</v>
       </c>
       <c r="F39" t="inlineStr">
@@ -1516,7 +1500,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K39" s="2" t="n">
+      <c r="K39" s="3" t="n">
         <v>665</v>
       </c>
       <c r="L39" t="inlineStr">
@@ -1564,7 +1548,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="3" t="n">
         <v>0.57</v>
       </c>
       <c r="D41" t="inlineStr">
@@ -1572,7 +1556,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="3" t="n">
         <v>0.42</v>
       </c>
       <c r="F41" t="inlineStr">
@@ -1592,7 +1576,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="3" t="n">
         <v>0.21</v>
       </c>
       <c r="F42" t="inlineStr">
@@ -1612,7 +1596,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>0.52</v>
       </c>
       <c r="D43" t="inlineStr">
@@ -1632,7 +1616,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <v>0.31</v>
       </c>
       <c r="D44" t="inlineStr">
@@ -1640,7 +1624,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="3" t="n">
         <v>0.29</v>
       </c>
       <c r="F44" t="inlineStr">
@@ -1660,7 +1644,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <v>0.43</v>
       </c>
       <c r="D45" t="inlineStr">
@@ -1668,7 +1652,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="3" t="n">
         <v>0.46</v>
       </c>
       <c r="F45" t="inlineStr">
@@ -1688,7 +1672,7 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E46" s="3" t="n">
         <v>0.31</v>
       </c>
       <c r="F46" t="inlineStr">
@@ -1708,7 +1692,7 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E47" s="2" t="n">
+      <c r="E47" s="3" t="n">
         <v>0.31</v>
       </c>
       <c r="F47" t="inlineStr">
@@ -1736,7 +1720,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E48" s="2" t="n">
+      <c r="E48" s="3" t="n">
         <v>0.72</v>
       </c>
       <c r="F48" t="inlineStr">
@@ -1744,7 +1728,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G48" s="3" t="n">
+      <c r="G48" s="2" t="n">
         <v>1.52</v>
       </c>
       <c r="H48" t="inlineStr">
@@ -1752,7 +1736,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="K48" s="2" t="n">
+      <c r="K48" s="3" t="n">
         <v>582.11</v>
       </c>
       <c r="L48" t="inlineStr">
@@ -1772,7 +1756,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E49" s="2" t="n">
+      <c r="E49" s="3" t="n">
         <v>0.26</v>
       </c>
       <c r="F49" t="inlineStr">
@@ -1800,7 +1784,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G50" s="2" t="n">
+      <c r="G50" s="3" t="n">
         <v>0.92</v>
       </c>
       <c r="H50" t="inlineStr">
@@ -1820,7 +1804,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
+      <c r="C51" s="3" t="n">
         <v>0.46</v>
       </c>
       <c r="D51" t="inlineStr">
@@ -1840,7 +1824,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E52" s="2" t="n">
+      <c r="E52" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F52" t="inlineStr">
@@ -1860,7 +1844,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E53" s="2" t="n">
+      <c r="E53" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F53" t="inlineStr">
@@ -1880,7 +1864,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E54" s="2" t="n">
+      <c r="E54" s="3" t="n">
         <v>0.31</v>
       </c>
       <c r="F54" t="inlineStr">
@@ -1888,7 +1872,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I54" s="3" t="n">
+      <c r="I54" s="2" t="n">
         <v>2098.51</v>
       </c>
       <c r="J54" t="inlineStr">
@@ -1897,7 +1881,7 @@
         </is>
       </c>
       <c r="K54" s="2" t="n">
-        <v>907.65</v>
+        <v>875.59</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -1916,7 +1900,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="C55" s="3" t="n">
+      <c r="C55" s="2" t="n">
         <v>1.68</v>
       </c>
       <c r="D55" t="inlineStr">
@@ -1924,7 +1908,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E55" s="2" t="n">
+      <c r="E55" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F55" t="inlineStr">
@@ -1932,7 +1916,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G55" s="3" t="n">
+      <c r="G55" s="2" t="n">
         <v>1.34</v>
       </c>
       <c r="H55" t="inlineStr">
@@ -1952,7 +1936,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" s="2" t="n">
         <v>1.6</v>
       </c>
       <c r="D56" t="inlineStr">
@@ -1960,7 +1944,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E56" s="2" t="n">
+      <c r="E56" s="3" t="n">
         <v>0.27</v>
       </c>
       <c r="F56" t="inlineStr">
@@ -1968,7 +1952,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G56" s="3" t="n">
+      <c r="G56" s="2" t="n">
         <v>1.26</v>
       </c>
       <c r="H56" t="inlineStr">
@@ -1988,7 +1972,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E57" s="2" t="n">
+      <c r="E57" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F57" t="inlineStr">
@@ -2008,7 +1992,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
+      <c r="C58" s="3" t="n">
         <v>0.45</v>
       </c>
       <c r="D58" t="inlineStr">
@@ -2016,7 +2000,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G58" s="2" t="n">
+      <c r="G58" s="3" t="n">
         <v>0.59</v>
       </c>
       <c r="H58" t="inlineStr">
@@ -2036,7 +2020,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="C59" s="2" t="n">
+      <c r="C59" s="3" t="n">
         <v>0.54</v>
       </c>
       <c r="D59" t="inlineStr">
@@ -2044,7 +2028,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E59" s="2" t="n">
+      <c r="E59" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F59" t="inlineStr">
@@ -2052,7 +2036,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G59" s="2" t="n">
+      <c r="G59" s="3" t="n">
         <v>0.8100000000000001</v>
       </c>
       <c r="H59" t="inlineStr">
@@ -2072,7 +2056,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E60" s="2" t="n">
+      <c r="E60" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F60" t="inlineStr">
@@ -2092,7 +2076,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="C61" s="2" t="n">
+      <c r="C61" s="3" t="n">
         <v>0.68</v>
       </c>
       <c r="D61" t="inlineStr">
@@ -2100,7 +2084,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E61" s="2" t="n">
+      <c r="E61" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F61" t="inlineStr">
@@ -2136,7 +2120,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E62" s="2" t="n">
+      <c r="E62" s="3" t="n">
         <v>0.32</v>
       </c>
       <c r="F62" t="inlineStr">
@@ -2156,7 +2140,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="C63" s="2" t="n">
+      <c r="C63" s="3" t="n">
         <v>0.34</v>
       </c>
       <c r="D63" t="inlineStr">
@@ -2164,7 +2148,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E63" s="2" t="n">
+      <c r="E63" s="3" t="n">
         <v>0.37</v>
       </c>
       <c r="F63" t="inlineStr">
@@ -2172,7 +2156,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G63" s="2" t="n">
+      <c r="G63" s="3" t="n">
         <v>0.77</v>
       </c>
       <c r="H63" t="inlineStr">
@@ -2188,14 +2172,6 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="K63" s="2" t="n">
-        <v>660.51</v>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2208,7 +2184,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E64" s="2" t="n">
+      <c r="E64" s="3" t="n">
         <v>0.38</v>
       </c>
       <c r="F64" t="inlineStr">
@@ -2216,12 +2192,20 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G64" s="3" t="n">
+      <c r="G64" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
           <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="n">
+        <v>633.84</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
@@ -2236,7 +2220,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E65" s="2" t="n">
+      <c r="E65" s="3" t="n">
         <v>0.37</v>
       </c>
       <c r="F65" t="inlineStr">
@@ -2256,7 +2240,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E66" s="2" t="n">
+      <c r="E66" s="3" t="n">
         <v>0.24</v>
       </c>
       <c r="F66" t="inlineStr">
@@ -2276,7 +2260,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="C67" s="2" t="n">
+      <c r="C67" s="3" t="n">
         <v>0.41</v>
       </c>
       <c r="D67" t="inlineStr">
@@ -2296,7 +2280,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C68" s="2" t="n">
+      <c r="C68" s="3" t="n">
         <v>0.27</v>
       </c>
       <c r="D68" t="inlineStr">
@@ -2316,20 +2300,12 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C69" s="2" t="n">
+      <c r="C69" s="3" t="n">
         <v>0.43</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
           <t>fp_higher</t>
-        </is>
-      </c>
-      <c r="K69" s="2" t="n">
-        <v>423.92</v>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2320,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C70" s="2" t="n">
+      <c r="C70" s="3" t="n">
         <v>0.7</v>
       </c>
       <c r="D70" t="inlineStr">
@@ -2352,7 +2328,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G70" s="2" t="n">
+      <c r="G70" s="3" t="n">
         <v>0.89</v>
       </c>
       <c r="H70" t="inlineStr">
@@ -2372,7 +2348,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C71" s="2" t="n">
+      <c r="C71" s="3" t="n">
         <v>0.18</v>
       </c>
       <c r="D71" t="inlineStr">
@@ -2392,7 +2368,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="C72" s="2" t="n">
+      <c r="C72" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="D72" t="inlineStr">
@@ -2412,7 +2388,7 @@
           <t>32</t>
         </is>
       </c>
-      <c r="E73" s="2" t="n">
+      <c r="E73" s="3" t="n">
         <v>0.21</v>
       </c>
       <c r="F73" t="inlineStr">
@@ -2432,7 +2408,7 @@
           <t>36</t>
         </is>
       </c>
-      <c r="C74" s="3" t="n">
+      <c r="C74" s="2" t="n">
         <v>1.01</v>
       </c>
       <c r="D74" t="inlineStr">
@@ -2460,7 +2436,7 @@
           <t>36</t>
         </is>
       </c>
-      <c r="C75" s="2" t="n">
+      <c r="C75" s="3" t="n">
         <v>0.43</v>
       </c>
       <c r="D75" t="inlineStr">
@@ -2468,7 +2444,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="I75" s="2" t="n">
+      <c r="I75" s="3" t="n">
         <v>452.54</v>
       </c>
       <c r="J75" t="inlineStr">
@@ -2488,7 +2464,7 @@
           <t>36</t>
         </is>
       </c>
-      <c r="C76" s="2" t="n">
+      <c r="C76" s="3" t="n">
         <v>0.65</v>
       </c>
       <c r="D76" t="inlineStr">
@@ -2536,7 +2512,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C78" s="2" t="n">
+      <c r="C78" s="3" t="n">
         <v>0.72</v>
       </c>
       <c r="D78" t="inlineStr">
@@ -2564,7 +2540,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C79" s="3" t="n">
+      <c r="C79" s="2" t="n">
         <v>1.33</v>
       </c>
       <c r="D79" t="inlineStr">
@@ -2572,7 +2548,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="E79" s="3" t="n">
+      <c r="E79" s="2" t="n">
         <v>1.27</v>
       </c>
       <c r="F79" t="inlineStr">
@@ -2592,7 +2568,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="E80" s="2" t="n">
+      <c r="E80" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F80" t="inlineStr">
@@ -2612,7 +2588,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C81" s="3" t="n">
+      <c r="C81" s="2" t="n">
         <v>2.06</v>
       </c>
       <c r="D81" t="inlineStr">
@@ -2620,7 +2596,7 @@
           <t>fp_higher</t>
         </is>
       </c>
-      <c r="G81" s="3" t="n">
+      <c r="G81" s="2" t="n">
         <v>1.86</v>
       </c>
       <c r="H81" t="inlineStr">
@@ -2640,7 +2616,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C82" s="3" t="n">
+      <c r="C82" s="2" t="n">
         <v>3.07</v>
       </c>
       <c r="D82" t="inlineStr">
@@ -2648,7 +2624,7 @@
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="E82" s="3" t="n">
+      <c r="E82" s="2" t="n">
         <v>3.11</v>
       </c>
       <c r="F82" t="inlineStr">
@@ -2668,7 +2644,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C83" s="3" t="n">
+      <c r="C83" s="2" t="n">
         <v>1.27</v>
       </c>
       <c r="D83" t="inlineStr">
@@ -2688,7 +2664,7 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E84" s="2" t="n">
+      <c r="E84" s="3" t="n">
         <v>0.26</v>
       </c>
       <c r="F84" t="inlineStr">
@@ -2708,18 +2684,10 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E85" s="2" t="n">
+      <c r="E85" s="3" t="n">
         <v>0.23</v>
       </c>
       <c r="F85" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K85" s="2" t="n">
-        <v>672.37</v>
-      </c>
-      <c r="L85" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2756,7 +2724,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E87" s="2" t="n">
+      <c r="E87" s="3" t="n">
         <v>0.18</v>
       </c>
       <c r="F87" t="inlineStr">
@@ -2776,7 +2744,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E88" s="2" t="n">
+      <c r="E88" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F88" t="inlineStr">
@@ -2804,7 +2772,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E89" s="2" t="n">
+      <c r="E89" s="3" t="n">
         <v>0.24</v>
       </c>
       <c r="F89" t="inlineStr">
@@ -2824,7 +2792,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E90" s="2" t="n">
+      <c r="E90" s="3" t="n">
         <v>0.2</v>
       </c>
       <c r="F90" t="inlineStr">
@@ -2844,7 +2812,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E91" s="2" t="n">
+      <c r="E91" s="3" t="n">
         <v>0.22</v>
       </c>
       <c r="F91" t="inlineStr">

</xml_diff>

<commit_message>
feat: Bland-Altman plots, correlation analysis, and p-value reporting
- Implement Bland-Altman plots for time and force measurements
- Calculate and display points within and outside limits of agreement
- Evaluate data quality based on points within limits of agreement
- Add correlation analysis with Pearson correlation coefficient and p-value
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -500,12 +500,12 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>t_con_force_diff</t>
+          <t>con_force_diff</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>t_con_force_comparison</t>
+          <t>con_force_comparison</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upt: more gymaware data added and updated scripts to work with gymaware data
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1964,16 +1964,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>26_bounce70b2</t>
+          <t>28_bounce70nb1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>28</t>
         </is>
       </c>
       <c r="E57" s="3" t="n">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -1984,26 +1984,18 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>26_bounce70b3</t>
+          <t>28_bounce70nb2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C58" s="3" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="G58" s="3" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="H58" t="inlineStr">
+          <t>28</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F58" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2012,118 +2004,86 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>26_bounce70nb1</t>
+          <t>28_bounce80nb3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C59" s="3" t="n">
-        <v>0.54</v>
+        <v>0.41</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E59" s="3" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="G59" s="3" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>26_bounce70nb2</t>
+          <t>29_bounce80b1</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="E60" s="3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>26_bounce70nb3</t>
+          <t>29_bounce80b2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C61" s="3" t="n">
-        <v>0.68</v>
+        <v>0.43</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>fp_higher</t>
-        </is>
-      </c>
-      <c r="E61" s="3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="I61" s="2" t="n">
-        <v>790.48</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K61" s="2" t="n">
-        <v>986.17</v>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>26_bounce80b1</t>
+          <t>29_bounce80nb1</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="E62" s="3" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="F62" t="inlineStr">
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="G62" s="3" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H62" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2132,96 +2092,56 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>26_bounce80b3</t>
+          <t>29_fastnb2</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C63" s="3" t="n">
-        <v>0.34</v>
+        <v>0.18</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E63" s="3" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="G63" s="3" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="I63" s="2" t="n">
-        <v>871.26</v>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>26_bounce80nb3</t>
+          <t>29_fastnb3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="E64" s="3" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
-        </is>
-      </c>
-      <c r="G64" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K64" s="3" t="n">
-        <v>633.84</v>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>28_bounce70nb1</t>
+          <t>32_bounce70nb3</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>32</t>
         </is>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.37</v>
+        <v>0.21</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -2232,18 +2152,26 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>28_bounce70nb2</t>
+          <t>36_fastnb1</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="E66" s="3" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="F66" t="inlineStr">
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="H66" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2252,18 +2180,26 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>28_bounce80nb3</t>
+          <t>36_fastnb3</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C67" s="3" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="D67" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="n">
+        <v>452.54</v>
+      </c>
+      <c r="J67" t="inlineStr">
         <is>
           <t>fp_higher</t>
         </is>
@@ -2272,38 +2208,46 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>29_bounce80b1</t>
+          <t>36_slownb1</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C68" s="3" t="n">
-        <v>0.27</v>
+        <v>0.65</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>fp_higher</t>
+          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>29_bounce80b2</t>
+          <t>38_bounce70nb1</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="C69" s="3" t="n">
-        <v>0.43</v>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>0.8100000000000001</v>
       </c>
       <c r="D69" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="F69" t="inlineStr">
         <is>
           <t>fp_higher</t>
         </is>
@@ -2312,46 +2256,54 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>29_bounce80nb1</t>
+          <t>38_bounce70nb3</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>38</t>
         </is>
       </c>
       <c r="C70" s="3" t="n">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G70" s="3" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
+      <c r="E70" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>29_fastnb2</t>
+          <t>38_bounce80nb1</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="n">
-        <v>0.18</v>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>1.33</v>
       </c>
       <c r="D71" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F71" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2360,18 +2312,18 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>29_fastnb3</t>
+          <t>38_fastnb2</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="C72" s="3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="D72" t="inlineStr">
+          <t>38</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="F72" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2380,74 +2332,74 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>32_bounce70nb3</t>
+          <t>38_slowb1</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="E73" s="3" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
+        </is>
+      </c>
+      <c r="G73" s="2" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>36_fastnb1</t>
+          <t>38_slownb2</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>38</t>
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>1.01</v>
+        <v>3.07</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
       </c>
-      <c r="G74" s="2" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
+      <c r="E74" s="2" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>36_fastnb3</t>
+          <t>38_slownb3</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="C75" s="3" t="n">
-        <v>0.43</v>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>1.27</v>
       </c>
       <c r="D75" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="I75" s="3" t="n">
-        <v>452.54</v>
-      </c>
-      <c r="J75" t="inlineStr">
         <is>
           <t>fp_higher</t>
         </is>
@@ -2456,18 +2408,18 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>36_slownb1</t>
+          <t>39_bounce70nb2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="C76" s="3" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="D76" t="inlineStr">
+          <t>39</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="F76" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>
@@ -2476,54 +2428,38 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>38_bounce70nb1</t>
+          <t>39_fastnb1</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C77" s="2" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E77" s="2" t="n">
-        <v>0.84</v>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>0.23</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>fp_higher</t>
+          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>38_bounce70nb3</t>
+          <t>39_slowb3</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C78" s="3" t="n">
-        <v>0.72</v>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>0.84</v>
       </c>
       <c r="D78" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="F78" t="inlineStr">
         <is>
           <t>fp_higher</t>
         </is>
@@ -2532,24 +2468,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>38_bounce80nb1</t>
+          <t>40_bounce70nb1</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C79" s="2" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
-        </is>
-      </c>
-      <c r="E79" s="2" t="n">
-        <v>1.27</v>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>0.18</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -2560,12 +2488,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>38_fastnb2</t>
+          <t>40_bounce70nb2</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E80" s="3" t="n">
@@ -2576,246 +2504,70 @@
           <t>gym_higher</t>
         </is>
       </c>
+      <c r="K80" s="2" t="n">
+        <v>835.33</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>38_slowb1</t>
+          <t>40_bounce80nb2</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C81" s="2" t="n">
-        <v>2.06</v>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
-        </is>
-      </c>
-      <c r="G81" s="2" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>38_slownb2</t>
+          <t>40_slownb1</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="n">
-        <v>3.07</v>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>3.11</v>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>0.2</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>fp_higher</t>
+          <t>gym_higher</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>38_slownb3</t>
+          <t>40_slownb3</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C83" s="2" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>39_bounce70nb2</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>39_fastnb1</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="E85" s="3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>39_slowb3</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>fp_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>40_bounce70nb1</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
           <t>40</t>
         </is>
       </c>
-      <c r="E87" s="3" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>40_bounce70nb2</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E88" s="3" t="n">
+      <c r="E83" s="3" t="n">
         <v>0.22</v>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="K88" s="2" t="n">
-        <v>835.33</v>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>40_bounce80nb2</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>40_slownb1</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E90" s="3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>40_slownb3</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="F91" t="inlineStr">
+      <c r="F83" t="inlineStr">
         <is>
           <t>gym_higher</t>
         </is>

</xml_diff>

<commit_message>
fix: Renamed Variables in all scripts
- turning_force --> F_turning
- con_force --> F_con
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -490,22 +490,22 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>turning_force_diff</t>
+          <t>F_turning_diff</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>turning_force_comparison</t>
+          <t>F_turning_comparison</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>con_force_diff</t>
+          <t>F_con_diff</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>con_force_comparison</t>
+          <t>F_con_comparison</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upt: variable renaming and validation
- F_con to peak_F_con
- updating validator to show separate time measruments
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -500,12 +500,12 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>F_con_diff</t>
+          <t>peak_F_con_diff</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>F_con_comparison</t>
+          <t>peak_F_con_comparison</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upt: Renamed Variables so it fits with paper
mean_F_con --> mFc
peak_F_con --> pFc
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -500,22 +500,22 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>peak_F_con_diff</t>
+          <t>pFc_diff</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>peak_F_con_comparison</t>
+          <t>pFc_comparison</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>mean_F_con_diff</t>
+          <t>mFc_diff</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>mean_F_con_comparison</t>
+          <t>mFc_comparison</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upt: Reverse engineered of GymAware pFc detection and applied to fp data, to validate FP
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N769"/>
+  <dimension ref="A1:P769"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,16 @@
           <t>mFc_comparison</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Fc_max_diff</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Fc_max_comparison</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -30594,18 +30604,34 @@
           <t>38</t>
         </is>
       </c>
-      <c r="C720" s="3" t="n">
-        <v>3.07</v>
+      <c r="C720" s="2" t="n">
+        <v>0.26</v>
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>gym_higher</t>
-        </is>
-      </c>
-      <c r="E720" s="3" t="n">
-        <v>3.11</v>
+          <t>fp_higher</t>
+        </is>
+      </c>
+      <c r="E720" s="2" t="n">
+        <v>0.22</v>
       </c>
       <c r="F720" t="inlineStr">
+        <is>
+          <t>gym_higher</t>
+        </is>
+      </c>
+      <c r="I720" s="2" t="n">
+        <v>92.63</v>
+      </c>
+      <c r="J720" t="inlineStr">
+        <is>
+          <t>fp_higher</t>
+        </is>
+      </c>
+      <c r="M720" s="2" t="n">
+        <v>182.24</v>
+      </c>
+      <c r="N720" t="inlineStr">
         <is>
           <t>fp_higher</t>
         </is>

</xml_diff>